<commit_message>
add spock test demo
</commit_message>
<xml_diff>
--- a/Auto test script.xlsx
+++ b/Auto test script.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pax-Exam" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="97">
   <si>
     <t xml:space="preserve"> - Là một maven project được xây dựng để test các module, bundle hay các chức năng nào đó trong môi trường OSGI</t>
   </si>
@@ -1556,12 +1556,21 @@
   <si>
     <t xml:space="preserve"> - Junit là một phần của họ kiến trúc xUnit dùng cho việc tạo các unit testing và test trong java</t>
   </si>
+  <si>
+    <t>2. Cách tạo spock test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Tham khảo:</t>
+  </si>
+  <si>
+    <t>https://code.google.com/p/spock/wiki/SpockBasics</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1677,6 +1686,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1775,10 +1791,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1807,8 +1827,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2148,7 +2170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2410,7 +2432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
@@ -3182,10 +3204,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3193,22 +3215,41 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="18.75">
+    <row r="2" spans="1:3" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="C9" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>